<commit_message>
filled out top level for giss-e2-1-cc
</commit_message>
<xml_diff>
--- a/cmip6/models/giss-e2-1-g-cc/cmip6_nasa-giss_giss-e2-1-g-cc_toplevel.xlsx
+++ b/cmip6/models/giss-e2-1-g-cc/cmip6_nasa-giss_giss-e2-1-g-cc_toplevel.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gaschmid/Desktop/nasa-giss/cmip6/models/giss-e2-1-g-cc/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{788117E6-4570-6A47-AFC6-12C3267EAF2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="7960" yWindow="3620" windowWidth="26740" windowHeight="16960" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Frontis" sheetId="1" r:id="rId1"/>
@@ -12,12 +18,12 @@
     <sheet name="1. Key Properties" sheetId="3" r:id="rId3"/>
     <sheet name="2. Radiative Forcings" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="784" uniqueCount="420">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="462">
   <si>
     <t>ES-DOC CMIP6 Model Documentation</t>
   </si>
@@ -37,7 +43,7 @@
     <t>Model</t>
   </si>
   <si>
-    <t>GISS-E2-1-G-CC</t>
+    <t>GISS-E2-1-G</t>
   </si>
   <si>
     <t>Realm / Topic</t>
@@ -1277,13 +1283,139 @@
   </si>
   <si>
     <t>cmip6.toplevel.radiative_forcings.other.solar.additional_information</t>
+  </si>
+  <si>
+    <t>Schmidt-Gavin</t>
+  </si>
+  <si>
+    <t>Principal Investigator</t>
+  </si>
+  <si>
+    <t>doi:10.1029/2019MS002025</t>
+  </si>
+  <si>
+    <t>NASA, GISS, Earth System Model</t>
+  </si>
+  <si>
+    <t>No flux corrections are used in the model.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GISS-E2-1-G is a modified version of GISS-E2-R with better tuning, improved parameterizations and increased upper ocean resolution. Description and evaluaiton is available in Kelley et al (2020, JAMES). </t>
+  </si>
+  <si>
+    <t>GISS-ER</t>
+  </si>
+  <si>
+    <t>GISS-E2-R</t>
+  </si>
+  <si>
+    <t>Please see the detailed description in Kelley et al (2020).</t>
+  </si>
+  <si>
+    <t>https://www.giss.nasa.gov/tools/modelE/</t>
+  </si>
+  <si>
+    <t>Fortran</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atmosphere, Ocean, Land, Sea ice, Vegetation, Land Ice are all components that are coupled together as described in Kelley et al (2020) and Schmidt et al (2014). </t>
+  </si>
+  <si>
+    <t>Atmospheric model is tuned for TOA energy balance with PI SST. Some tuning related to low and high clouds for match to climatological radiative fluxes, and gravity wave drag for stratospheric-tropospheric exchange and high latitude SLP.  Full description in Kelley et al (2020).</t>
+  </si>
+  <si>
+    <t>TOA OLW, TOA ASW, SLP</t>
+  </si>
+  <si>
+    <t>THC</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Atmospheric model independently with PI SST. Ocean mixing within coupled model to reduce OHC drift in PI coupled control. </t>
+  </si>
+  <si>
+    <t>Each component is fully water mass conserving. No further effort was required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Heat is conserved in every component. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ocean accepts natural boundary conditions (so water mass, salt, heat) and is mass conserving (not volume conserving). </t>
+  </si>
+  <si>
+    <t>All heat fluxes are conserved.</t>
+  </si>
+  <si>
+    <t>Heat is conserved. Sea ice uses a conservative brine pocket formation (Bitz and Lipscomp, 1999; Schmidt et al, 2004).</t>
+  </si>
+  <si>
+    <t>Heat, salt and water mass is conserved. Sea ice uses a conservative brine pocket formation (Bitz and Lipscomp, 1999; Schmidt et al, 2004).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rivers carry water mass and heat which is input directly and naturally into the ocean at the river mouth. Net heat/mass imbalance over ice sheets is distributed to ocean using a fixed area mask separately for the NH (around Greenland) and SH (around Antarctic). Effective glacial runoff (ice and heat) is entered into the ocean over the top 700 meters.  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fresh water is conserved throughout the model (with the very small exception of the chemical source of H2O in the stratosphere from the oxidation of CH4). </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precip, evaporation are added/removed from the ocean naturally. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Precip, evaporation is added/removed from soils/lakes/rivers. </t>
+  </si>
+  <si>
+    <t>Precip/sublimation is added/removed from sea ice.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">River runoff is added to the ocean naturally at the river outlet. Glacial runoff likewise. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Net mass loss from ice sheets (which in the real world would be iceberg calving) is spread around Greenland and Antarctica (independently) to maintain total water mass balance.  </t>
+  </si>
+  <si>
+    <t>Water accumulates or not. If lakes start to fill, they expand using a fixed geometry until the evaporation matches the runoff. If no balance can be found, the endoreic basin have special river directions that will kick in once a specific lake level is reached.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Snow accumulates and evaporates/metls according to a snow model. If snow accumulates indefinitely, than the excess snow is added to the glacial mass being added around Greenland or Antarctica depending on hemisphere. </t>
+  </si>
+  <si>
+    <t>Salt is conserved. Total salt is maintained as a conserved variable in both sea ice and ocean.</t>
+  </si>
+  <si>
+    <t>Momentum is conserved in surface fluxes and through atmospheric mixing and GWD.</t>
+  </si>
+  <si>
+    <t>No idea what this question means.</t>
+  </si>
+  <si>
+    <t>This depends on the physics-version and experiment. p1 uses Y, p3 and p5 use ES in the historical simulations and E in the future scenarios.</t>
+  </si>
+  <si>
+    <t>This depends on the physics-version and experiment. p1 uses Y derived from the p3 AMIP simulations and future scenarios. P3 and p5 use E in the historical simulations and future scenarios.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EESC is determined as 2.19*(CFC11 + CFC12) plus background </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Depends on phsyics version. In p1 AIE is tuned to provide -1 W/m2 based on imposed aerosol concentration. In p3, AIE is parameterized. In p5 it's more complicated. </t>
+  </si>
+  <si>
+    <t>This depends on the physics-version and experiment. p1 uses constant  C derived from the p3 AMIP simulations and future scenarios. P3 and p5 use E in the historical simulations and future scenarios.</t>
+  </si>
+  <si>
+    <t>land use includes changes to crops, pasture and irrigation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Historical runs are driven by changes in well-mixed GHGs (CO2, CH4, N2O, CFC-11, CFC-12, and other CFCs), aerosol changes (including indirect effects on clouds and on snow albedo, ozone changes, solar spectral irradiance, volcanic aerosols, and orbital variations. Land uce /land cover change includes irrigation which have radiative impacts at the surface.  Thie model version has an interactive ocean-land-atmosphere carbon cycle, and so CO2 is driven by emissions and feedbacks to natural fluxes. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="15">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1384,6 +1516,12 @@
       <name val="Helvetica Neue"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1429,7 +1567,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1473,12 +1611,21 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1525,7 +1672,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1557,9 +1704,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1591,6 +1756,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1766,24 +1949,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="35.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="180.7109375" style="1" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="35.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="180.6640625" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="33" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
@@ -1791,7 +1974,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1799,7 +1982,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
@@ -1807,7 +1990,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -1815,7 +1998,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>9</v>
       </c>
@@ -1823,12 +2006,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
+    <row r="9" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="B9" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="11" spans="1:2">
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
@@ -1836,7 +2019,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:2">
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="5" t="s">
         <v>14</v>
       </c>
@@ -1844,7 +2027,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A13" s="5" t="s">
         <v>16</v>
       </c>
@@ -1852,7 +2035,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="14" spans="1:2">
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A14" s="5" t="s">
         <v>18</v>
       </c>
@@ -1860,13 +2043,13 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="B16" s="4"/>
     </row>
-    <row r="17" spans="1:2">
+    <row r="17" spans="1:2" ht="20" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>21</v>
       </c>
@@ -1874,54 +2057,56 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B11" r:id="rId1"/>
-    <hyperlink ref="B12" r:id="rId2"/>
+    <hyperlink ref="B11" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B12" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:B17"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="80.7109375" customWidth="1"/>
-    <col min="2" max="2" width="40.7109375" customWidth="1"/>
-    <col min="3" max="16384" width="9.140625" style="6"/>
+    <col min="1" max="1" width="80.6640625" customWidth="1"/>
+    <col min="2" max="2" width="40.6640625" customWidth="1"/>
+    <col min="3" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>22</v>
       </c>
       <c r="B1" s="7"/>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="9"/>
     </row>
-    <row r="6" spans="1:2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="8" spans="1:2">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="10" t="s">
         <v>27</v>
       </c>
@@ -1929,27 +2114,31 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="11"/>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="12" spans="1:2">
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A9" s="11" t="s">
+        <v>420</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>29</v>
       </c>
       <c r="B12" s="9"/>
     </row>
-    <row r="13" spans="1:2">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:2">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="16" spans="1:2">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="10" t="s">
         <v>27</v>
       </c>
@@ -1957,42 +2146,48 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2">
-      <c r="A17" s="11"/>
-      <c r="B17" s="11"/>
+    <row r="17" spans="1:2" ht="19" x14ac:dyDescent="0.2">
+      <c r="A17" s="15" t="s">
+        <v>422</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>8</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B9" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Author,Contributor,Principal Investigator,Point of Contact,Sponsor"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B17" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"Top Level,Key Properties,Radiative Forcings"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" r:id="rId1"/>
-    <hyperlink ref="A13" r:id="rId2"/>
+    <hyperlink ref="A6" r:id="rId1" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink ref="A13" r:id="rId2" xr:uid="{00000000-0004-0000-0100-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD224"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:AH224"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A216" workbookViewId="0">
+      <selection activeCell="B224" sqref="B224"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>17</v>
       </c>
@@ -2000,12 +2195,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>35</v>
       </c>
@@ -2013,7 +2208,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -2024,10 +2219,12 @@
         <v>39</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>40</v>
       </c>
@@ -2035,7 +2232,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>37</v>
       </c>
@@ -2046,15 +2243,17 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="24" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="13" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>45</v>
       </c>
@@ -2062,7 +2261,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="14" t="s">
         <v>37</v>
       </c>
@@ -2073,15 +2272,17 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="178" customHeight="1">
-      <c r="B16" s="11"/>
-    </row>
-    <row r="19" spans="1:3" ht="24" customHeight="1">
+    <row r="16" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B16" s="11" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="12" t="s">
         <v>50</v>
       </c>
@@ -2089,12 +2290,12 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="24" customHeight="1">
+    <row r="20" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B20" s="13" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="24" customHeight="1">
+    <row r="22" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>53</v>
       </c>
@@ -2102,7 +2303,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="24" customHeight="1">
+    <row r="23" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -2113,15 +2314,17 @@
         <v>56</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="24" customHeight="1">
+    <row r="24" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="178" customHeight="1">
-      <c r="B25" s="11"/>
-    </row>
-    <row r="28" spans="1:3" ht="24" customHeight="1">
+    <row r="25" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B25" s="11" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>57</v>
       </c>
@@ -2129,12 +2332,12 @@
         <v>58</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="24" customHeight="1">
+    <row r="29" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="24" customHeight="1">
+    <row r="31" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>60</v>
       </c>
@@ -2142,7 +2345,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="24" customHeight="1">
+    <row r="32" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>37</v>
       </c>
@@ -2153,10 +2356,12 @@
         <v>63</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="24" customHeight="1">
-      <c r="B33" s="11"/>
-    </row>
-    <row r="35" spans="1:3" ht="24" customHeight="1">
+    <row r="33" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B33" s="11">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="9" t="s">
         <v>64</v>
       </c>
@@ -2164,7 +2369,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="24" customHeight="1">
+    <row r="36" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="14" t="s">
         <v>37</v>
       </c>
@@ -2175,10 +2380,12 @@
         <v>67</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="24" customHeight="1">
-      <c r="B37" s="11"/>
-    </row>
-    <row r="39" spans="1:3" ht="24" customHeight="1">
+    <row r="37" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B37" s="11" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="9" t="s">
         <v>68</v>
       </c>
@@ -2186,7 +2393,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="24" customHeight="1">
+    <row r="40" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="14" t="s">
         <v>37</v>
       </c>
@@ -2197,10 +2404,12 @@
         <v>71</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="24" customHeight="1">
-      <c r="B41" s="11"/>
-    </row>
-    <row r="43" spans="1:3" ht="24" customHeight="1">
+    <row r="41" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="9" t="s">
         <v>72</v>
       </c>
@@ -2208,7 +2417,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="24" customHeight="1">
+    <row r="44" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="14" t="s">
         <v>37</v>
       </c>
@@ -2219,15 +2428,17 @@
         <v>75</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="24" customHeight="1">
+    <row r="45" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B45" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="178" customHeight="1">
-      <c r="B46" s="11"/>
-    </row>
-    <row r="48" spans="1:3" ht="24" customHeight="1">
+    <row r="46" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="11" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>76</v>
       </c>
@@ -2235,7 +2446,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="24" customHeight="1">
+    <row r="49" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="14" t="s">
         <v>37</v>
       </c>
@@ -2246,10 +2457,10 @@
         <v>79</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="24" customHeight="1">
+    <row r="50" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B50" s="11"/>
     </row>
-    <row r="53" spans="1:3" ht="24" customHeight="1">
+    <row r="53" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="12" t="s">
         <v>80</v>
       </c>
@@ -2257,12 +2468,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="24" customHeight="1">
+    <row r="54" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B54" s="13" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="24" customHeight="1">
+    <row r="56" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>83</v>
       </c>
@@ -2270,7 +2481,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="24" customHeight="1">
+    <row r="57" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="14" t="s">
         <v>37</v>
       </c>
@@ -2281,10 +2492,12 @@
         <v>86</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="24" customHeight="1">
-      <c r="B58" s="11"/>
-    </row>
-    <row r="60" spans="1:3" ht="24" customHeight="1">
+    <row r="58" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B58" s="11" t="s">
+        <v>429</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="9" t="s">
         <v>87</v>
       </c>
@@ -2292,7 +2505,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="24" customHeight="1">
+    <row r="61" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="14" t="s">
         <v>37</v>
       </c>
@@ -2303,10 +2516,10 @@
         <v>90</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="24" customHeight="1">
+    <row r="62" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B62" s="11"/>
     </row>
-    <row r="64" spans="1:3" ht="24" customHeight="1">
+    <row r="64" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>91</v>
       </c>
@@ -2314,7 +2527,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="65" spans="1:34" ht="24" customHeight="1">
+    <row r="65" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="14" t="s">
         <v>37</v>
       </c>
@@ -2325,15 +2538,17 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="1:34" ht="24" customHeight="1">
+    <row r="66" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B66" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="67" spans="1:34" ht="24" customHeight="1">
-      <c r="B67" s="11"/>
-    </row>
-    <row r="69" spans="1:34" ht="24" customHeight="1">
+    <row r="67" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="11" t="s">
+        <v>430</v>
+      </c>
+    </row>
+    <row r="69" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>95</v>
       </c>
@@ -2341,7 +2556,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="70" spans="1:34" ht="24" customHeight="1">
+    <row r="70" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="14" t="s">
         <v>37</v>
       </c>
@@ -2352,10 +2567,12 @@
         <v>98</v>
       </c>
     </row>
-    <row r="71" spans="1:34" ht="24" customHeight="1">
-      <c r="B71" s="11"/>
-    </row>
-    <row r="73" spans="1:34" ht="24" customHeight="1">
+    <row r="71" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B71" s="11" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="73" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>99</v>
       </c>
@@ -2363,7 +2580,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:34" ht="24" customHeight="1">
+    <row r="74" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="14" t="s">
         <v>101</v>
       </c>
@@ -2374,8 +2591,10 @@
         <v>103</v>
       </c>
     </row>
-    <row r="75" spans="1:34" ht="24" customHeight="1">
-      <c r="B75" s="11"/>
+    <row r="75" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="11" t="s">
+        <v>108</v>
+      </c>
       <c r="AA75" s="6" t="s">
         <v>104</v>
       </c>
@@ -2401,7 +2620,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:34" ht="24" customHeight="1">
+    <row r="78" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="12" t="s">
         <v>112</v>
       </c>
@@ -2409,10 +2628,10 @@
         <v>113</v>
       </c>
     </row>
-    <row r="79" spans="1:34" ht="24" customHeight="1">
+    <row r="79" spans="1:34" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B79" s="13"/>
     </row>
-    <row r="81" spans="1:30" ht="24" customHeight="1">
+    <row r="81" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>114</v>
       </c>
@@ -2420,7 +2639,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="82" spans="1:30" ht="24" customHeight="1">
+    <row r="82" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="14" t="s">
         <v>116</v>
       </c>
@@ -2431,10 +2650,12 @@
         <v>118</v>
       </c>
     </row>
-    <row r="83" spans="1:30" ht="24" customHeight="1">
-      <c r="B83" s="11"/>
-    </row>
-    <row r="85" spans="1:30" ht="24" customHeight="1">
+    <row r="83" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B83" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>119</v>
       </c>
@@ -2442,7 +2663,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="24" customHeight="1">
+    <row r="86" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="14" t="s">
         <v>101</v>
       </c>
@@ -2453,8 +2674,10 @@
         <v>122</v>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="24" customHeight="1">
-      <c r="B87" s="11"/>
+    <row r="87" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B87" s="11" t="s">
+        <v>123</v>
+      </c>
       <c r="AA87" s="6" t="s">
         <v>123</v>
       </c>
@@ -2468,7 +2691,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="24" customHeight="1">
+    <row r="89" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="9" t="s">
         <v>126</v>
       </c>
@@ -2476,7 +2699,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="24" customHeight="1">
+    <row r="90" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="14" t="s">
         <v>116</v>
       </c>
@@ -2487,10 +2710,12 @@
         <v>129</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="24" customHeight="1">
-      <c r="B91" s="11"/>
-    </row>
-    <row r="94" spans="1:30" ht="24" customHeight="1">
+    <row r="91" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B91" s="11" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="94" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="12" t="s">
         <v>130</v>
       </c>
@@ -2498,12 +2723,12 @@
         <v>131</v>
       </c>
     </row>
-    <row r="95" spans="1:30" ht="24" customHeight="1">
+    <row r="95" spans="1:30" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B95" s="13" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="97" spans="1:3" ht="24" customHeight="1">
+    <row r="97" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="9" t="s">
         <v>133</v>
       </c>
@@ -2511,7 +2736,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="98" spans="1:3" ht="24" customHeight="1">
+    <row r="98" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="14" t="s">
         <v>37</v>
       </c>
@@ -2522,15 +2747,17 @@
         <v>136</v>
       </c>
     </row>
-    <row r="99" spans="1:3" ht="24" customHeight="1">
+    <row r="99" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B99" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="100" spans="1:3" ht="178" customHeight="1">
-      <c r="B100" s="11"/>
-    </row>
-    <row r="102" spans="1:3" ht="24" customHeight="1">
+    <row r="100" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B100" s="11" t="s">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>137</v>
       </c>
@@ -2538,7 +2765,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:3" ht="24" customHeight="1">
+    <row r="103" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="14" t="s">
         <v>37</v>
       </c>
@@ -2549,15 +2776,17 @@
         <v>140</v>
       </c>
     </row>
-    <row r="104" spans="1:3" ht="24" customHeight="1">
+    <row r="104" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B104" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="105" spans="1:3" ht="24" customHeight="1">
-      <c r="B105" s="11"/>
-    </row>
-    <row r="107" spans="1:3" ht="24" customHeight="1">
+    <row r="105" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B105" s="11" t="s">
+        <v>433</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="9" t="s">
         <v>141</v>
       </c>
@@ -2565,7 +2794,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="108" spans="1:3" ht="24" customHeight="1">
+    <row r="108" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="14" t="s">
         <v>37</v>
       </c>
@@ -2576,15 +2805,17 @@
         <v>144</v>
       </c>
     </row>
-    <row r="109" spans="1:3" ht="24" customHeight="1">
+    <row r="109" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B109" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="110" spans="1:3" ht="24" customHeight="1">
-      <c r="B110" s="11"/>
-    </row>
-    <row r="112" spans="1:3" ht="24" customHeight="1">
+    <row r="110" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B110" s="11" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
         <v>145</v>
       </c>
@@ -2592,7 +2823,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="113" spans="1:3" ht="24" customHeight="1">
+    <row r="113" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="14" t="s">
         <v>37</v>
       </c>
@@ -2603,15 +2834,17 @@
         <v>148</v>
       </c>
     </row>
-    <row r="114" spans="1:3" ht="24" customHeight="1">
+    <row r="114" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B114" s="8" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="115" spans="1:3" ht="24" customHeight="1">
-      <c r="B115" s="11"/>
-    </row>
-    <row r="117" spans="1:3" ht="24" customHeight="1">
+    <row r="115" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B115" s="11" t="s">
+        <v>435</v>
+      </c>
+    </row>
+    <row r="117" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="9" t="s">
         <v>149</v>
       </c>
@@ -2619,7 +2852,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="118" spans="1:3" ht="24" customHeight="1">
+    <row r="118" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="14" t="s">
         <v>37</v>
       </c>
@@ -2630,10 +2863,12 @@
         <v>152</v>
       </c>
     </row>
-    <row r="119" spans="1:3" ht="24" customHeight="1">
-      <c r="B119" s="11"/>
-    </row>
-    <row r="121" spans="1:3" ht="24" customHeight="1">
+    <row r="119" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B119" s="11" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="121" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="9" t="s">
         <v>153</v>
       </c>
@@ -2641,7 +2876,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="122" spans="1:3" ht="24" customHeight="1">
+    <row r="122" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="14" t="s">
         <v>37</v>
       </c>
@@ -2652,10 +2887,12 @@
         <v>156</v>
       </c>
     </row>
-    <row r="123" spans="1:3" ht="24" customHeight="1">
-      <c r="B123" s="11"/>
-    </row>
-    <row r="126" spans="1:3" ht="24" customHeight="1">
+    <row r="123" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B123" s="11" t="s">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="126" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A126" s="12" t="s">
         <v>157</v>
       </c>
@@ -2663,12 +2900,12 @@
         <v>158</v>
       </c>
     </row>
-    <row r="127" spans="1:3" ht="24" customHeight="1">
+    <row r="127" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B127" s="13" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="129" spans="1:3" ht="24" customHeight="1">
+    <row r="129" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="9" t="s">
         <v>160</v>
       </c>
@@ -2676,7 +2913,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="130" spans="1:3" ht="24" customHeight="1">
+    <row r="130" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="14" t="s">
         <v>37</v>
       </c>
@@ -2687,15 +2924,17 @@
         <v>163</v>
       </c>
     </row>
-    <row r="131" spans="1:3" ht="24" customHeight="1">
+    <row r="131" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B131" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="132" spans="1:3" ht="178" customHeight="1">
-      <c r="B132" s="11"/>
-    </row>
-    <row r="134" spans="1:3" ht="24" customHeight="1">
+    <row r="132" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="11" t="s">
+        <v>438</v>
+      </c>
+    </row>
+    <row r="134" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="9" t="s">
         <v>164</v>
       </c>
@@ -2703,7 +2942,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="135" spans="1:3" ht="24" customHeight="1">
+    <row r="135" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="14" t="s">
         <v>37</v>
       </c>
@@ -2714,15 +2953,17 @@
         <v>167</v>
       </c>
     </row>
-    <row r="136" spans="1:3" ht="24" customHeight="1">
+    <row r="136" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B136" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="1:3" ht="178" customHeight="1">
-      <c r="B137" s="11"/>
-    </row>
-    <row r="139" spans="1:3" ht="24" customHeight="1">
+    <row r="137" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B137" s="11" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="139" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="9" t="s">
         <v>168</v>
       </c>
@@ -2730,7 +2971,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="140" spans="1:3" ht="24" customHeight="1">
+    <row r="140" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="14" t="s">
         <v>37</v>
       </c>
@@ -2741,15 +2982,17 @@
         <v>171</v>
       </c>
     </row>
-    <row r="141" spans="1:3" ht="24" customHeight="1">
+    <row r="141" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B141" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="1:3" ht="178" customHeight="1">
-      <c r="B142" s="11"/>
-    </row>
-    <row r="144" spans="1:3" ht="24" customHeight="1">
+    <row r="142" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B142" s="11" t="s">
+        <v>440</v>
+      </c>
+    </row>
+    <row r="144" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="9" t="s">
         <v>172</v>
       </c>
@@ -2757,7 +3000,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="145" spans="1:3" ht="24" customHeight="1">
+    <row r="145" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="14" t="s">
         <v>37</v>
       </c>
@@ -2768,15 +3011,17 @@
         <v>175</v>
       </c>
     </row>
-    <row r="146" spans="1:3" ht="24" customHeight="1">
+    <row r="146" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B146" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="1:3" ht="178" customHeight="1">
-      <c r="B147" s="11"/>
-    </row>
-    <row r="149" spans="1:3" ht="24" customHeight="1">
+    <row r="147" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B147" s="11" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="149" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="9" t="s">
         <v>176</v>
       </c>
@@ -2784,7 +3029,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="150" spans="1:3" ht="24" customHeight="1">
+    <row r="150" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="14" t="s">
         <v>37</v>
       </c>
@@ -2795,15 +3040,17 @@
         <v>179</v>
       </c>
     </row>
-    <row r="151" spans="1:3" ht="24" customHeight="1">
+    <row r="151" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="178" customHeight="1">
-      <c r="B152" s="11"/>
-    </row>
-    <row r="154" spans="1:3" ht="24" customHeight="1">
+    <row r="152" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B152" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="154" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="9" t="s">
         <v>180</v>
       </c>
@@ -2811,7 +3058,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="155" spans="1:3" ht="24" customHeight="1">
+    <row r="155" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="14" t="s">
         <v>37</v>
       </c>
@@ -2822,15 +3069,17 @@
         <v>183</v>
       </c>
     </row>
-    <row r="156" spans="1:3" ht="24" customHeight="1">
+    <row r="156" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B156" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="157" spans="1:3" ht="178" customHeight="1">
-      <c r="B157" s="11"/>
-    </row>
-    <row r="160" spans="1:3" ht="24" customHeight="1">
+    <row r="157" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B157" s="11" t="s">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="160" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A160" s="12" t="s">
         <v>184</v>
       </c>
@@ -2838,12 +3087,12 @@
         <v>185</v>
       </c>
     </row>
-    <row r="161" spans="1:3" ht="24" customHeight="1">
+    <row r="161" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B161" s="13" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="163" spans="1:3" ht="24" customHeight="1">
+    <row r="163" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A163" s="9" t="s">
         <v>187</v>
       </c>
@@ -2851,7 +3100,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="164" spans="1:3" ht="24" customHeight="1">
+    <row r="164" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A164" s="14" t="s">
         <v>37</v>
       </c>
@@ -2862,15 +3111,17 @@
         <v>189</v>
       </c>
     </row>
-    <row r="165" spans="1:3" ht="24" customHeight="1">
+    <row r="165" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B165" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="166" spans="1:3" ht="178" customHeight="1">
-      <c r="B166" s="11"/>
-    </row>
-    <row r="168" spans="1:3" ht="24" customHeight="1">
+    <row r="166" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B166" s="11" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="168" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A168" s="9" t="s">
         <v>190</v>
       </c>
@@ -2878,7 +3129,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="169" spans="1:3" ht="24" customHeight="1">
+    <row r="169" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A169" s="14" t="s">
         <v>37</v>
       </c>
@@ -2889,15 +3140,17 @@
         <v>192</v>
       </c>
     </row>
-    <row r="170" spans="1:3" ht="24" customHeight="1">
+    <row r="170" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B170" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="171" spans="1:3" ht="178" customHeight="1">
-      <c r="B171" s="11"/>
-    </row>
-    <row r="173" spans="1:3" ht="24" customHeight="1">
+    <row r="171" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B171" s="11" t="s">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="173" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A173" s="9" t="s">
         <v>193</v>
       </c>
@@ -2905,7 +3158,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="174" spans="1:3" ht="24" customHeight="1">
+    <row r="174" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A174" s="14" t="s">
         <v>37</v>
       </c>
@@ -2916,15 +3169,17 @@
         <v>195</v>
       </c>
     </row>
-    <row r="175" spans="1:3" ht="24" customHeight="1">
+    <row r="175" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B175" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="176" spans="1:3" ht="178" customHeight="1">
-      <c r="B176" s="11"/>
-    </row>
-    <row r="178" spans="1:3" ht="24" customHeight="1">
+    <row r="176" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B176" s="11" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A178" s="9" t="s">
         <v>196</v>
       </c>
@@ -2932,7 +3187,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="179" spans="1:3" ht="24" customHeight="1">
+    <row r="179" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A179" s="14" t="s">
         <v>37</v>
       </c>
@@ -2943,15 +3198,17 @@
         <v>198</v>
       </c>
     </row>
-    <row r="180" spans="1:3" ht="24" customHeight="1">
+    <row r="180" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B180" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="181" spans="1:3" ht="178" customHeight="1">
-      <c r="B181" s="11"/>
-    </row>
-    <row r="183" spans="1:3" ht="24" customHeight="1">
+    <row r="181" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B181" s="11" t="s">
+        <v>447</v>
+      </c>
+    </row>
+    <row r="183" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A183" s="9" t="s">
         <v>199</v>
       </c>
@@ -2959,7 +3216,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="184" spans="1:3" ht="24" customHeight="1">
+    <row r="184" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A184" s="14" t="s">
         <v>37</v>
       </c>
@@ -2970,15 +3227,17 @@
         <v>201</v>
       </c>
     </row>
-    <row r="185" spans="1:3" ht="24" customHeight="1">
+    <row r="185" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B185" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="186" spans="1:3" ht="178" customHeight="1">
-      <c r="B186" s="11"/>
-    </row>
-    <row r="188" spans="1:3" ht="24" customHeight="1">
+    <row r="186" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B186" s="11" t="s">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="188" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A188" s="9" t="s">
         <v>202</v>
       </c>
@@ -2986,7 +3245,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="189" spans="1:3" ht="24" customHeight="1">
+    <row r="189" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A189" s="14" t="s">
         <v>37</v>
       </c>
@@ -2997,15 +3256,17 @@
         <v>205</v>
       </c>
     </row>
-    <row r="190" spans="1:3" ht="24" customHeight="1">
+    <row r="190" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B190" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="191" spans="1:3" ht="178" customHeight="1">
-      <c r="B191" s="11"/>
-    </row>
-    <row r="193" spans="1:3" ht="24" customHeight="1">
+    <row r="191" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B191" s="11" t="s">
+        <v>448</v>
+      </c>
+    </row>
+    <row r="193" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A193" s="9" t="s">
         <v>206</v>
       </c>
@@ -3013,7 +3274,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="194" spans="1:3" ht="24" customHeight="1">
+    <row r="194" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A194" s="14" t="s">
         <v>37</v>
       </c>
@@ -3024,15 +3285,17 @@
         <v>209</v>
       </c>
     </row>
-    <row r="195" spans="1:3" ht="24" customHeight="1">
+    <row r="195" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B195" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="196" spans="1:3" ht="178" customHeight="1">
-      <c r="B196" s="11"/>
-    </row>
-    <row r="198" spans="1:3" ht="24" customHeight="1">
+    <row r="196" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B196" s="11" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="198" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A198" s="9" t="s">
         <v>210</v>
       </c>
@@ -3040,7 +3303,7 @@
         <v>211</v>
       </c>
     </row>
-    <row r="199" spans="1:3" ht="24" customHeight="1">
+    <row r="199" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A199" s="14" t="s">
         <v>37</v>
       </c>
@@ -3051,15 +3314,17 @@
         <v>213</v>
       </c>
     </row>
-    <row r="200" spans="1:3" ht="24" customHeight="1">
+    <row r="200" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B200" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="201" spans="1:3" ht="178" customHeight="1">
-      <c r="B201" s="11"/>
-    </row>
-    <row r="203" spans="1:3" ht="24" customHeight="1">
+    <row r="201" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B201" s="11" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="203" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A203" s="9" t="s">
         <v>214</v>
       </c>
@@ -3067,7 +3332,7 @@
         <v>215</v>
       </c>
     </row>
-    <row r="204" spans="1:3" ht="24" customHeight="1">
+    <row r="204" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A204" s="14" t="s">
         <v>37</v>
       </c>
@@ -3078,15 +3343,17 @@
         <v>217</v>
       </c>
     </row>
-    <row r="205" spans="1:3" ht="24" customHeight="1">
+    <row r="205" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B205" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="206" spans="1:3" ht="178" customHeight="1">
-      <c r="B206" s="11"/>
-    </row>
-    <row r="209" spans="1:3" ht="24" customHeight="1">
+    <row r="206" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B206" s="11" t="s">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="209" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A209" s="12" t="s">
         <v>218</v>
       </c>
@@ -3094,12 +3361,12 @@
         <v>219</v>
       </c>
     </row>
-    <row r="210" spans="1:3" ht="24" customHeight="1">
+    <row r="210" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B210" s="13" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="212" spans="1:3" ht="24" customHeight="1">
+    <row r="212" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A212" s="9" t="s">
         <v>221</v>
       </c>
@@ -3107,7 +3374,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="213" spans="1:3" ht="24" customHeight="1">
+    <row r="213" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A213" s="14" t="s">
         <v>37</v>
       </c>
@@ -3118,15 +3385,17 @@
         <v>223</v>
       </c>
     </row>
-    <row r="214" spans="1:3" ht="24" customHeight="1">
+    <row r="214" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B214" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="215" spans="1:3" ht="178" customHeight="1">
-      <c r="B215" s="11"/>
-    </row>
-    <row r="218" spans="1:3" ht="24" customHeight="1">
+    <row r="215" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B215" s="11" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="218" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A218" s="12" t="s">
         <v>224</v>
       </c>
@@ -3134,12 +3403,12 @@
         <v>225</v>
       </c>
     </row>
-    <row r="219" spans="1:3" ht="24" customHeight="1">
+    <row r="219" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B219" s="13" t="s">
         <v>226</v>
       </c>
     </row>
-    <row r="221" spans="1:3" ht="24" customHeight="1">
+    <row r="221" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A221" s="9" t="s">
         <v>227</v>
       </c>
@@ -3147,7 +3416,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="222" spans="1:3" ht="24" customHeight="1">
+    <row r="222" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A222" s="14" t="s">
         <v>37</v>
       </c>
@@ -3158,27 +3427,26 @@
         <v>229</v>
       </c>
     </row>
-    <row r="223" spans="1:3" ht="24" customHeight="1">
+    <row r="223" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B223" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="224" spans="1:3" ht="178" customHeight="1">
-      <c r="B224" s="11"/>
+    <row r="224" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B224" s="11" t="s">
+        <v>453</v>
+      </c>
     </row>
   </sheetData>
-  <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75">
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B75" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>AA75:AH75</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B83 B91" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B87" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>AA87:AD87</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B91">
-      <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3186,20 +3454,22 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:XFD299"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:AG306"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="150.7109375" customWidth="1"/>
+    <col min="1" max="1" width="13.6640625" customWidth="1"/>
+    <col min="2" max="2" width="150.6640625" customWidth="1"/>
     <col min="3" max="3" width="0" hidden="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="6"/>
+    <col min="4" max="16384" width="9.1640625" style="6"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24" customHeight="1">
+    <row r="1" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="12" t="s">
         <v>230</v>
       </c>
@@ -3207,12 +3477,12 @@
         <v>231</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="24" customHeight="1">
+    <row r="2" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B2" s="13" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="24" customHeight="1">
+    <row r="4" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="9" t="s">
         <v>233</v>
       </c>
@@ -3220,7 +3490,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="24" customHeight="1">
+    <row r="5" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="14" t="s">
         <v>37</v>
       </c>
@@ -3231,10 +3501,12 @@
         <v>235</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="24" customHeight="1">
-      <c r="B6" s="11"/>
-    </row>
-    <row r="8" spans="1:3" ht="24" customHeight="1">
+    <row r="6" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B6" s="11" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="9" t="s">
         <v>236</v>
       </c>
@@ -3242,7 +3514,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="24" customHeight="1">
+    <row r="9" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="14" t="s">
         <v>37</v>
       </c>
@@ -3253,15 +3525,17 @@
         <v>238</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="24" customHeight="1">
+    <row r="10" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="178" customHeight="1">
-      <c r="B11" s="11"/>
-    </row>
-    <row r="14" spans="1:3" ht="24" customHeight="1">
+    <row r="11" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B11" s="11" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="12" t="s">
         <v>239</v>
       </c>
@@ -3269,12 +3543,12 @@
         <v>240</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="24" customHeight="1">
+    <row r="15" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B15" s="13" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="17" spans="1:33" ht="24" customHeight="1">
+    <row r="17" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>242</v>
       </c>
@@ -3282,7 +3556,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="18" spans="1:33" ht="24" customHeight="1">
+    <row r="18" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="14" t="s">
         <v>101</v>
       </c>
@@ -3293,13 +3567,15 @@
         <v>245</v>
       </c>
     </row>
-    <row r="19" spans="1:33" ht="24" customHeight="1">
+    <row r="19" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B19" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="20" spans="1:33" ht="24" customHeight="1">
-      <c r="B20" s="11"/>
+    <row r="20" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B20" s="11" t="s">
+        <v>249</v>
+      </c>
       <c r="AA20" s="6" t="s">
         <v>246</v>
       </c>
@@ -3322,7 +3598,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="22" spans="1:33" ht="24" customHeight="1">
+    <row r="22" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="9" t="s">
         <v>252</v>
       </c>
@@ -3330,7 +3606,7 @@
         <v>253</v>
       </c>
     </row>
-    <row r="23" spans="1:33" ht="24" customHeight="1">
+    <row r="23" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="14" t="s">
         <v>37</v>
       </c>
@@ -3341,15 +3617,15 @@
         <v>255</v>
       </c>
     </row>
-    <row r="24" spans="1:33" ht="24" customHeight="1">
+    <row r="24" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B24" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:33" ht="178" customHeight="1">
+    <row r="25" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B25" s="11"/>
     </row>
-    <row r="28" spans="1:33" ht="24" customHeight="1">
+    <row r="28" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="12" t="s">
         <v>256</v>
       </c>
@@ -3357,12 +3633,12 @@
         <v>257</v>
       </c>
     </row>
-    <row r="29" spans="1:33" ht="24" customHeight="1">
+    <row r="29" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B29" s="13" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="31" spans="1:33" ht="24" customHeight="1">
+    <row r="31" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="9" t="s">
         <v>259</v>
       </c>
@@ -3370,7 +3646,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:33" ht="24" customHeight="1">
+    <row r="32" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="14" t="s">
         <v>101</v>
       </c>
@@ -3381,13 +3657,15 @@
         <v>260</v>
       </c>
     </row>
-    <row r="33" spans="1:33" ht="24" customHeight="1">
+    <row r="33" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B33" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="34" spans="1:33" ht="24" customHeight="1">
-      <c r="B34" s="11"/>
+    <row r="34" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B34" s="11" t="s">
+        <v>248</v>
+      </c>
       <c r="AA34" s="6" t="s">
         <v>246</v>
       </c>
@@ -3410,1805 +3688,1978 @@
         <v>111</v>
       </c>
     </row>
-    <row r="36" spans="1:33" ht="24" customHeight="1">
-      <c r="A36" s="9" t="s">
+    <row r="35" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA35" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB35" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC35" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD35" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE35" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF35" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG35" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B36" s="11" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA36" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB36" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC36" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD36" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE36" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF36" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG36" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="9" t="s">
         <v>261</v>
       </c>
-      <c r="B36" s="9" t="s">
+      <c r="B38" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="37" spans="1:33" ht="24" customHeight="1">
-      <c r="A37" s="14" t="s">
+    <row r="39" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B37" s="10" t="s">
+      <c r="B39" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C37" s="10" t="s">
+      <c r="C39" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="38" spans="1:33" ht="24" customHeight="1">
-      <c r="B38" s="8" t="s">
+    <row r="40" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B40" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="39" spans="1:33" ht="178" customHeight="1">
-      <c r="B39" s="11"/>
-    </row>
-    <row r="42" spans="1:33" ht="24" customHeight="1">
-      <c r="A42" s="12" t="s">
+    <row r="41" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B41" s="11" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="44" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="12" t="s">
         <v>263</v>
       </c>
-      <c r="B42" s="12" t="s">
+      <c r="B44" s="12" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="43" spans="1:33" ht="24" customHeight="1">
-      <c r="B43" s="13" t="s">
+    <row r="45" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="13" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="45" spans="1:33" ht="24" customHeight="1">
-      <c r="A45" s="9" t="s">
+    <row r="47" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="46" spans="1:33" ht="24" customHeight="1">
-      <c r="A46" s="14" t="s">
+    <row r="48" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B46" s="10" t="s">
+      <c r="B48" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C46" s="10" t="s">
+      <c r="C48" s="10" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="47" spans="1:33" ht="24" customHeight="1">
-      <c r="B47" s="10" t="s">
+    <row r="49" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B49" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="48" spans="1:33" ht="24" customHeight="1">
-      <c r="B48" s="11"/>
-      <c r="AA48" s="6" t="s">
+    <row r="50" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B50" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA50" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB48" s="6" t="s">
+      <c r="AB50" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC48" s="6" t="s">
+      <c r="AC50" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD48" s="6" t="s">
+      <c r="AD50" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE48" s="6" t="s">
+      <c r="AE50" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF48" s="6" t="s">
+      <c r="AF50" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG48" s="6" t="s">
+      <c r="AG50" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="50" spans="1:33" ht="24" customHeight="1">
-      <c r="A50" s="9" t="s">
+    <row r="52" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="9" t="s">
         <v>268</v>
       </c>
-      <c r="B50" s="9" t="s">
+      <c r="B52" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="51" spans="1:33" ht="24" customHeight="1">
-      <c r="A51" s="14" t="s">
+    <row r="53" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B51" s="10" t="s">
+      <c r="B53" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C51" s="10" t="s">
+      <c r="C53" s="10" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="52" spans="1:33" ht="24" customHeight="1">
-      <c r="B52" s="8" t="s">
+    <row r="54" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B54" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:33" ht="178" customHeight="1">
-      <c r="B53" s="11"/>
-    </row>
-    <row r="56" spans="1:33" ht="24" customHeight="1">
-      <c r="A56" s="12" t="s">
+    <row r="55" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B55" s="11"/>
+    </row>
+    <row r="58" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="12" t="s">
         <v>270</v>
       </c>
-      <c r="B56" s="12" t="s">
+      <c r="B58" s="12" t="s">
         <v>271</v>
       </c>
     </row>
-    <row r="57" spans="1:33" ht="24" customHeight="1">
-      <c r="B57" s="13" t="s">
+    <row r="59" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B59" s="13" t="s">
         <v>272</v>
       </c>
     </row>
-    <row r="59" spans="1:33" ht="24" customHeight="1">
-      <c r="A59" s="9" t="s">
+    <row r="61" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="9" t="s">
         <v>273</v>
       </c>
-      <c r="B59" s="9" t="s">
+      <c r="B61" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="60" spans="1:33" ht="24" customHeight="1">
-      <c r="A60" s="14" t="s">
+    <row r="62" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B60" s="10" t="s">
+      <c r="B62" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C62" s="10" t="s">
         <v>274</v>
       </c>
     </row>
-    <row r="61" spans="1:33" ht="24" customHeight="1">
-      <c r="B61" s="10" t="s">
+    <row r="63" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B63" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="62" spans="1:33" ht="24" customHeight="1">
-      <c r="B62" s="11"/>
-      <c r="AA62" s="6" t="s">
+    <row r="64" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B64" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA64" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB62" s="6" t="s">
+      <c r="AB64" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC62" s="6" t="s">
+      <c r="AC64" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD62" s="6" t="s">
+      <c r="AD64" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE62" s="6" t="s">
+      <c r="AE64" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF62" s="6" t="s">
+      <c r="AF64" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG62" s="6" t="s">
+      <c r="AG64" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="64" spans="1:33" ht="24" customHeight="1">
-      <c r="A64" s="9" t="s">
+    <row r="65" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B65" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA65" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB65" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC65" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD65" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE65" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF65" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG65" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="67" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="9" t="s">
         <v>275</v>
       </c>
-      <c r="B64" s="9" t="s">
+      <c r="B67" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="65" spans="1:33" ht="24" customHeight="1">
-      <c r="A65" s="14" t="s">
+    <row r="68" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B65" s="10" t="s">
+      <c r="B68" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C65" s="10" t="s">
+      <c r="C68" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="66" spans="1:33" ht="24" customHeight="1">
-      <c r="B66" s="8" t="s">
+    <row r="69" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="67" spans="1:33" ht="178" customHeight="1">
-      <c r="B67" s="11"/>
-    </row>
-    <row r="70" spans="1:33" ht="24" customHeight="1">
-      <c r="A70" s="12" t="s">
+    <row r="70" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="73" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="12" t="s">
         <v>277</v>
       </c>
-      <c r="B70" s="12" t="s">
+      <c r="B73" s="12" t="s">
         <v>278</v>
       </c>
     </row>
-    <row r="71" spans="1:33" ht="24" customHeight="1">
-      <c r="B71" s="13" t="s">
+    <row r="74" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B74" s="13" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="73" spans="1:33" ht="24" customHeight="1">
-      <c r="A73" s="9" t="s">
+    <row r="76" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="9" t="s">
         <v>280</v>
       </c>
-      <c r="B73" s="9" t="s">
+      <c r="B76" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="74" spans="1:33" ht="24" customHeight="1">
-      <c r="A74" s="14" t="s">
+    <row r="77" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A77" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B74" s="10" t="s">
+      <c r="B77" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C74" s="10" t="s">
+      <c r="C77" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="75" spans="1:33" ht="24" customHeight="1">
-      <c r="B75" s="10" t="s">
+    <row r="78" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B78" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="76" spans="1:33" ht="24" customHeight="1">
-      <c r="B76" s="11"/>
-      <c r="AA76" s="6" t="s">
+    <row r="79" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B79" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA79" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB76" s="6" t="s">
+      <c r="AB79" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC76" s="6" t="s">
+      <c r="AC79" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD76" s="6" t="s">
+      <c r="AD79" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE76" s="6" t="s">
+      <c r="AE79" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF76" s="6" t="s">
+      <c r="AF79" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG76" s="6" t="s">
+      <c r="AG79" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="78" spans="1:33" ht="24" customHeight="1">
-      <c r="A78" s="9" t="s">
+    <row r="80" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B80" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA80" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB80" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC80" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD80" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE80" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF80" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG80" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="82" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A82" s="9" t="s">
         <v>282</v>
       </c>
-      <c r="B78" s="9" t="s">
+      <c r="B82" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="79" spans="1:33" ht="24" customHeight="1">
-      <c r="A79" s="14" t="s">
+    <row r="83" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A83" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B79" s="10" t="s">
+      <c r="B83" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C79" s="10" t="s">
+      <c r="C83" s="10" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="80" spans="1:33" ht="24" customHeight="1">
-      <c r="B80" s="8" t="s">
+    <row r="84" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B84" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="81" spans="1:33" ht="178" customHeight="1">
-      <c r="B81" s="11"/>
-    </row>
-    <row r="84" spans="1:33" ht="24" customHeight="1">
-      <c r="A84" s="12" t="s">
+    <row r="85" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B85" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="88" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A88" s="12" t="s">
         <v>284</v>
       </c>
-      <c r="B84" s="12" t="s">
+      <c r="B88" s="12" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="85" spans="1:33" ht="24" customHeight="1">
-      <c r="B85" s="13" t="s">
+    <row r="89" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="13" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="87" spans="1:33" ht="24" customHeight="1">
-      <c r="A87" s="9" t="s">
+    <row r="91" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A91" s="9" t="s">
         <v>287</v>
       </c>
-      <c r="B87" s="9" t="s">
+      <c r="B91" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="88" spans="1:33" ht="24" customHeight="1">
-      <c r="A88" s="14" t="s">
+    <row r="92" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A92" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B92" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C88" s="10" t="s">
+      <c r="C92" s="10" t="s">
         <v>288</v>
       </c>
     </row>
-    <row r="89" spans="1:33" ht="24" customHeight="1">
-      <c r="B89" s="10" t="s">
+    <row r="93" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B93" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="90" spans="1:33" ht="24" customHeight="1">
-      <c r="B90" s="11"/>
-      <c r="AA90" s="6" t="s">
+    <row r="94" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B94" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA94" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB90" s="6" t="s">
+      <c r="AB94" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC90" s="6" t="s">
+      <c r="AC94" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD90" s="6" t="s">
+      <c r="AD94" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE90" s="6" t="s">
+      <c r="AE94" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF90" s="6" t="s">
+      <c r="AF94" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG90" s="6" t="s">
+      <c r="AG94" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="92" spans="1:33" ht="24" customHeight="1">
-      <c r="A92" s="9" t="s">
+    <row r="96" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A96" s="9" t="s">
         <v>289</v>
       </c>
-      <c r="B92" s="9" t="s">
+      <c r="B96" s="9" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="93" spans="1:33" ht="24" customHeight="1">
-      <c r="A93" s="14" t="s">
+    <row r="97" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A97" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B97" s="10" t="s">
         <v>291</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C97" s="10" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="94" spans="1:33" ht="24" customHeight="1">
-      <c r="B94" s="11"/>
-      <c r="AA94" s="6" t="s">
+    <row r="98" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B98" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA98" s="6" t="s">
         <v>293</v>
       </c>
-      <c r="AB94" s="6" t="s">
+      <c r="AB98" s="6" t="s">
         <v>294</v>
       </c>
-      <c r="AC94" s="6" t="s">
+      <c r="AC98" s="6" t="s">
         <v>295</v>
       </c>
-      <c r="AD94" s="6" t="s">
+      <c r="AD98" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="AE94" s="6" t="s">
+      <c r="AE98" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="96" spans="1:33" ht="24" customHeight="1">
-      <c r="A96" s="9" t="s">
+    <row r="100" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A100" s="9" t="s">
         <v>297</v>
       </c>
-      <c r="B96" s="9" t="s">
+      <c r="B100" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="97" spans="1:33" ht="24" customHeight="1">
-      <c r="A97" s="14" t="s">
+    <row r="101" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A101" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B101" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C101" s="10" t="s">
         <v>298</v>
       </c>
     </row>
-    <row r="98" spans="1:33" ht="24" customHeight="1">
-      <c r="B98" s="8" t="s">
+    <row r="102" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B102" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="99" spans="1:33" ht="178" customHeight="1">
-      <c r="B99" s="11"/>
-    </row>
-    <row r="102" spans="1:33" ht="24" customHeight="1">
-      <c r="A102" s="12" t="s">
+    <row r="103" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B103" s="11" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="106" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A106" s="12" t="s">
         <v>299</v>
       </c>
-      <c r="B102" s="12" t="s">
+      <c r="B106" s="12" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="103" spans="1:33" ht="24" customHeight="1">
-      <c r="B103" s="13" t="s">
+    <row r="107" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B107" s="13" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="105" spans="1:33" ht="24" customHeight="1">
-      <c r="A105" s="9" t="s">
+    <row r="109" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A109" s="9" t="s">
         <v>302</v>
       </c>
-      <c r="B105" s="9" t="s">
+      <c r="B109" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="106" spans="1:33" ht="24" customHeight="1">
-      <c r="A106" s="14" t="s">
+    <row r="110" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A110" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B110" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C110" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="107" spans="1:33" ht="24" customHeight="1">
-      <c r="B107" s="10" t="s">
+    <row r="111" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B111" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="108" spans="1:33" ht="24" customHeight="1">
-      <c r="B108" s="11"/>
-      <c r="AA108" s="6" t="s">
+    <row r="112" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B112" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA112" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB108" s="6" t="s">
+      <c r="AB112" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC108" s="6" t="s">
+      <c r="AC112" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD108" s="6" t="s">
+      <c r="AD112" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE108" s="6" t="s">
+      <c r="AE112" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF108" s="6" t="s">
+      <c r="AF112" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG108" s="6" t="s">
+      <c r="AG112" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="110" spans="1:33" ht="24" customHeight="1">
-      <c r="A110" s="9" t="s">
+    <row r="114" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A114" s="9" t="s">
         <v>304</v>
       </c>
-      <c r="B110" s="9" t="s">
+      <c r="B114" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="111" spans="1:33" ht="24" customHeight="1">
-      <c r="A111" s="14" t="s">
+    <row r="115" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A115" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="B115" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C111" s="10" t="s">
+      <c r="C115" s="10" t="s">
         <v>305</v>
       </c>
     </row>
-    <row r="112" spans="1:33" ht="24" customHeight="1">
-      <c r="B112" s="8" t="s">
+    <row r="116" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B116" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="113" spans="1:33" ht="178" customHeight="1">
-      <c r="B113" s="11"/>
-    </row>
-    <row r="116" spans="1:33" ht="24" customHeight="1">
-      <c r="A116" s="12" t="s">
+    <row r="117" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B117" s="11"/>
+    </row>
+    <row r="120" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A120" s="12" t="s">
         <v>306</v>
       </c>
-      <c r="B116" s="12" t="s">
+      <c r="B120" s="12" t="s">
         <v>307</v>
       </c>
     </row>
-    <row r="117" spans="1:33" ht="24" customHeight="1">
-      <c r="B117" s="13" t="s">
+    <row r="121" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B121" s="13" t="s">
         <v>308</v>
       </c>
     </row>
-    <row r="119" spans="1:33" ht="24" customHeight="1">
-      <c r="A119" s="9" t="s">
+    <row r="123" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A123" s="9" t="s">
         <v>309</v>
       </c>
-      <c r="B119" s="9" t="s">
+      <c r="B123" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="120" spans="1:33" ht="24" customHeight="1">
-      <c r="A120" s="14" t="s">
+    <row r="124" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A124" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B120" s="10" t="s">
+      <c r="B124" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C120" s="10" t="s">
+      <c r="C124" s="10" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="121" spans="1:33" ht="24" customHeight="1">
-      <c r="B121" s="10" t="s">
+    <row r="125" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B125" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="122" spans="1:33" ht="24" customHeight="1">
-      <c r="B122" s="11"/>
-      <c r="AA122" s="6" t="s">
+    <row r="126" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B126" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA126" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB122" s="6" t="s">
+      <c r="AB126" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC122" s="6" t="s">
+      <c r="AC126" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD122" s="6" t="s">
+      <c r="AD126" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE122" s="6" t="s">
+      <c r="AE126" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF122" s="6" t="s">
+      <c r="AF126" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG122" s="6" t="s">
+      <c r="AG126" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="124" spans="1:33" ht="24" customHeight="1">
-      <c r="A124" s="9" t="s">
+    <row r="127" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B127" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA127" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB127" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC127" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD127" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE127" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF127" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG127" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="129" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A129" s="9" t="s">
         <v>311</v>
       </c>
-      <c r="B124" s="9" t="s">
+      <c r="B129" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="125" spans="1:33" ht="24" customHeight="1">
-      <c r="A125" s="14" t="s">
+    <row r="130" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A130" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B125" s="10" t="s">
+      <c r="B130" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C125" s="10" t="s">
+      <c r="C130" s="10" t="s">
         <v>312</v>
       </c>
     </row>
-    <row r="126" spans="1:33" ht="24" customHeight="1">
-      <c r="B126" s="8" t="s">
+    <row r="131" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B131" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:33" ht="178" customHeight="1">
-      <c r="B127" s="11"/>
-    </row>
-    <row r="130" spans="1:33" ht="24" customHeight="1">
-      <c r="A130" s="12" t="s">
+    <row r="132" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B132" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="135" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A135" s="12" t="s">
         <v>313</v>
       </c>
-      <c r="B130" s="12" t="s">
+      <c r="B135" s="12" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="131" spans="1:33" ht="24" customHeight="1">
-      <c r="B131" s="13" t="s">
+    <row r="136" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B136" s="13" t="s">
         <v>315</v>
       </c>
     </row>
-    <row r="133" spans="1:33" ht="24" customHeight="1">
-      <c r="A133" s="9" t="s">
+    <row r="138" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A138" s="9" t="s">
         <v>316</v>
       </c>
-      <c r="B133" s="9" t="s">
+      <c r="B138" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="134" spans="1:33" ht="24" customHeight="1">
-      <c r="A134" s="14" t="s">
+    <row r="139" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A139" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B134" s="10" t="s">
+      <c r="B139" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C134" s="10" t="s">
+      <c r="C139" s="10" t="s">
         <v>317</v>
       </c>
     </row>
-    <row r="135" spans="1:33" ht="24" customHeight="1">
-      <c r="B135" s="10" t="s">
+    <row r="140" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B140" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="136" spans="1:33" ht="24" customHeight="1">
-      <c r="B136" s="11"/>
-      <c r="AA136" s="6" t="s">
+    <row r="141" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B141" s="11"/>
+      <c r="AA141" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB136" s="6" t="s">
+      <c r="AB141" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC136" s="6" t="s">
+      <c r="AC141" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD136" s="6" t="s">
+      <c r="AD141" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE136" s="6" t="s">
+      <c r="AE141" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF136" s="6" t="s">
+      <c r="AF141" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG136" s="6" t="s">
+      <c r="AG141" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="138" spans="1:33" ht="24" customHeight="1">
-      <c r="A138" s="9" t="s">
+    <row r="143" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A143" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="B138" s="9" t="s">
+      <c r="B143" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="139" spans="1:33" ht="24" customHeight="1">
-      <c r="A139" s="14" t="s">
+    <row r="144" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A144" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B139" s="10" t="s">
+      <c r="B144" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C139" s="10" t="s">
+      <c r="C144" s="10" t="s">
         <v>319</v>
       </c>
     </row>
-    <row r="140" spans="1:33" ht="24" customHeight="1">
-      <c r="B140" s="8" t="s">
+    <row r="145" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B145" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="1:33" ht="178" customHeight="1">
-      <c r="B141" s="11"/>
-    </row>
-    <row r="144" spans="1:33" ht="24" customHeight="1">
-      <c r="A144" s="12" t="s">
+    <row r="146" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B146" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="149" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A149" s="12" t="s">
         <v>320</v>
       </c>
-      <c r="B144" s="12" t="s">
+      <c r="B149" s="12" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="145" spans="1:33" ht="24" customHeight="1">
-      <c r="B145" s="13" t="s">
+    <row r="150" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B150" s="13" t="s">
         <v>322</v>
       </c>
     </row>
-    <row r="147" spans="1:33" ht="24" customHeight="1">
-      <c r="A147" s="9" t="s">
+    <row r="152" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A152" s="9" t="s">
         <v>323</v>
       </c>
-      <c r="B147" s="9" t="s">
+      <c r="B152" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="148" spans="1:33" ht="24" customHeight="1">
-      <c r="A148" s="14" t="s">
+    <row r="153" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A153" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B148" s="10" t="s">
+      <c r="B153" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C148" s="10" t="s">
+      <c r="C153" s="10" t="s">
         <v>324</v>
       </c>
     </row>
-    <row r="149" spans="1:33" ht="24" customHeight="1">
-      <c r="B149" s="10" t="s">
+    <row r="154" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B154" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="150" spans="1:33" ht="24" customHeight="1">
-      <c r="B150" s="11"/>
-      <c r="AA150" s="6" t="s">
+    <row r="155" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B155" s="11"/>
+      <c r="AA155" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB150" s="6" t="s">
+      <c r="AB155" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC150" s="6" t="s">
+      <c r="AC155" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD150" s="6" t="s">
+      <c r="AD155" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE150" s="6" t="s">
+      <c r="AE155" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF150" s="6" t="s">
+      <c r="AF155" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG150" s="6" t="s">
+      <c r="AG155" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="152" spans="1:33" ht="24" customHeight="1">
-      <c r="A152" s="9" t="s">
+    <row r="157" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A157" s="9" t="s">
         <v>325</v>
       </c>
-      <c r="B152" s="9" t="s">
+      <c r="B157" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="153" spans="1:33" ht="24" customHeight="1">
-      <c r="A153" s="14" t="s">
+    <row r="158" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A158" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B153" s="10" t="s">
+      <c r="B158" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C153" s="10" t="s">
+      <c r="C158" s="10" t="s">
         <v>326</v>
       </c>
     </row>
-    <row r="154" spans="1:33" ht="24" customHeight="1">
-      <c r="B154" s="8" t="s">
+    <row r="159" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B159" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="155" spans="1:33" ht="178" customHeight="1">
-      <c r="B155" s="11"/>
-    </row>
-    <row r="158" spans="1:33" ht="24" customHeight="1">
-      <c r="A158" s="12" t="s">
+    <row r="160" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B160" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="163" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A163" s="12" t="s">
         <v>327</v>
       </c>
-      <c r="B158" s="12" t="s">
+      <c r="B163" s="12" t="s">
         <v>328</v>
       </c>
     </row>
-    <row r="159" spans="1:33" ht="24" customHeight="1">
-      <c r="B159" s="13" t="s">
+    <row r="164" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B164" s="13" t="s">
         <v>329</v>
       </c>
     </row>
-    <row r="161" spans="1:33" ht="24" customHeight="1">
-      <c r="A161" s="9" t="s">
+    <row r="166" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A166" s="9" t="s">
         <v>330</v>
       </c>
-      <c r="B161" s="9" t="s">
+      <c r="B166" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="162" spans="1:33" ht="24" customHeight="1">
-      <c r="A162" s="14" t="s">
+    <row r="167" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A167" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B162" s="10" t="s">
+      <c r="B167" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C162" s="10" t="s">
+      <c r="C167" s="10" t="s">
         <v>331</v>
       </c>
     </row>
-    <row r="163" spans="1:33" ht="24" customHeight="1">
-      <c r="B163" s="10" t="s">
+    <row r="168" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B168" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="164" spans="1:33" ht="24" customHeight="1">
-      <c r="B164" s="11"/>
-      <c r="AA164" s="6" t="s">
+    <row r="169" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B169" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="AA169" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB164" s="6" t="s">
+      <c r="AB169" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC164" s="6" t="s">
+      <c r="AC169" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD164" s="6" t="s">
+      <c r="AD169" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE164" s="6" t="s">
+      <c r="AE169" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF164" s="6" t="s">
+      <c r="AF169" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG164" s="6" t="s">
+      <c r="AG169" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="166" spans="1:33" ht="24" customHeight="1">
-      <c r="A166" s="9" t="s">
+    <row r="171" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A171" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="B166" s="9" t="s">
+      <c r="B171" s="9" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="167" spans="1:33" ht="24" customHeight="1">
-      <c r="A167" s="14" t="s">
+    <row r="172" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A172" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B167" s="10" t="s">
+      <c r="B172" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C167" s="10" t="s">
+      <c r="C172" s="10" t="s">
         <v>335</v>
       </c>
     </row>
-    <row r="168" spans="1:33" ht="24" customHeight="1">
-      <c r="B168" s="11"/>
-    </row>
-    <row r="170" spans="1:33" ht="24" customHeight="1">
-      <c r="A170" s="9" t="s">
+    <row r="173" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B173" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="175" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A175" s="9" t="s">
         <v>336</v>
       </c>
-      <c r="B170" s="9" t="s">
+      <c r="B175" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="171" spans="1:33" ht="24" customHeight="1">
-      <c r="A171" s="14" t="s">
+    <row r="176" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A176" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B171" s="10" t="s">
+      <c r="B176" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C171" s="10" t="s">
+      <c r="C176" s="10" t="s">
         <v>337</v>
       </c>
     </row>
-    <row r="172" spans="1:33" ht="24" customHeight="1">
-      <c r="B172" s="8" t="s">
+    <row r="177" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B177" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="173" spans="1:33" ht="178" customHeight="1">
-      <c r="B173" s="11"/>
-    </row>
-    <row r="176" spans="1:33" ht="24" customHeight="1">
-      <c r="A176" s="12" t="s">
+    <row r="178" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B178" s="11" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="181" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A181" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="B176" s="12" t="s">
+      <c r="B181" s="12" t="s">
         <v>339</v>
       </c>
     </row>
-    <row r="177" spans="1:33" ht="24" customHeight="1">
-      <c r="B177" s="13" t="s">
+    <row r="182" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B182" s="13" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="179" spans="1:33" ht="24" customHeight="1">
-      <c r="A179" s="9" t="s">
+    <row r="184" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A184" s="9" t="s">
         <v>341</v>
       </c>
-      <c r="B179" s="9" t="s">
+      <c r="B184" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="180" spans="1:33" ht="24" customHeight="1">
-      <c r="A180" s="14" t="s">
+    <row r="185" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A185" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B180" s="10" t="s">
+      <c r="B185" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C180" s="10" t="s">
+      <c r="C185" s="10" t="s">
         <v>342</v>
       </c>
     </row>
-    <row r="181" spans="1:33" ht="24" customHeight="1">
-      <c r="B181" s="10" t="s">
+    <row r="186" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B186" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="182" spans="1:33" ht="24" customHeight="1">
-      <c r="B182" s="11"/>
-      <c r="AA182" s="6" t="s">
+    <row r="187" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B187" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="AB182" s="6" t="s">
+      <c r="AA187" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB187" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC182" s="6" t="s">
+      <c r="AC187" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD182" s="6" t="s">
+      <c r="AD187" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE182" s="6" t="s">
+      <c r="AE187" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF182" s="6" t="s">
+      <c r="AF187" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG182" s="6" t="s">
+      <c r="AG187" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="184" spans="1:33" ht="24" customHeight="1">
-      <c r="A184" s="9" t="s">
+    <row r="189" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A189" s="9" t="s">
         <v>343</v>
       </c>
-      <c r="B184" s="9" t="s">
+      <c r="B189" s="9" t="s">
         <v>333</v>
       </c>
     </row>
-    <row r="185" spans="1:33" ht="24" customHeight="1">
-      <c r="A185" s="14" t="s">
+    <row r="190" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A190" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B185" s="10" t="s">
+      <c r="B190" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="C185" s="10" t="s">
+      <c r="C190" s="10" t="s">
         <v>344</v>
       </c>
     </row>
-    <row r="186" spans="1:33" ht="24" customHeight="1">
-      <c r="B186" s="11"/>
-    </row>
-    <row r="188" spans="1:33" ht="24" customHeight="1">
-      <c r="A188" s="9" t="s">
+    <row r="191" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B191" s="11"/>
+    </row>
+    <row r="193" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A193" s="9" t="s">
         <v>345</v>
       </c>
-      <c r="B188" s="9" t="s">
+      <c r="B193" s="9" t="s">
         <v>346</v>
       </c>
     </row>
-    <row r="189" spans="1:33" ht="24" customHeight="1">
-      <c r="A189" s="14" t="s">
+    <row r="194" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A194" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B189" s="10" t="s">
+      <c r="B194" s="10" t="s">
         <v>347</v>
       </c>
-      <c r="C189" s="10" t="s">
+      <c r="C194" s="10" t="s">
         <v>348</v>
       </c>
     </row>
-    <row r="190" spans="1:33" ht="24" customHeight="1">
-      <c r="B190" s="11"/>
-    </row>
-    <row r="192" spans="1:33" ht="24" customHeight="1">
-      <c r="A192" s="9" t="s">
+    <row r="195" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B195" s="11"/>
+    </row>
+    <row r="197" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A197" s="9" t="s">
         <v>349</v>
       </c>
-      <c r="B192" s="9" t="s">
+      <c r="B197" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="193" spans="1:33" ht="24" customHeight="1">
-      <c r="A193" s="14" t="s">
+    <row r="198" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A198" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B193" s="10" t="s">
+      <c r="B198" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C193" s="10" t="s">
+      <c r="C198" s="10" t="s">
         <v>350</v>
       </c>
     </row>
-    <row r="194" spans="1:33" ht="24" customHeight="1">
-      <c r="B194" s="8" t="s">
+    <row r="199" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B199" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="195" spans="1:33" ht="178" customHeight="1">
-      <c r="B195" s="11"/>
-    </row>
-    <row r="198" spans="1:33" ht="24" customHeight="1">
-      <c r="A198" s="12" t="s">
+    <row r="200" spans="1:3" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B200" s="11"/>
+    </row>
+    <row r="203" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A203" s="12" t="s">
         <v>351</v>
       </c>
-      <c r="B198" s="12" t="s">
+      <c r="B203" s="12" t="s">
         <v>352</v>
       </c>
     </row>
-    <row r="199" spans="1:33" ht="24" customHeight="1">
-      <c r="B199" s="13" t="s">
+    <row r="204" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B204" s="13" t="s">
         <v>353</v>
       </c>
     </row>
-    <row r="201" spans="1:33" ht="24" customHeight="1">
-      <c r="A201" s="9" t="s">
+    <row r="206" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A206" s="9" t="s">
         <v>354</v>
       </c>
-      <c r="B201" s="9" t="s">
+      <c r="B206" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="202" spans="1:33" ht="24" customHeight="1">
-      <c r="A202" s="14" t="s">
+    <row r="207" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A207" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B202" s="10" t="s">
+      <c r="B207" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C202" s="10" t="s">
+      <c r="C207" s="10" t="s">
         <v>355</v>
       </c>
     </row>
-    <row r="203" spans="1:33" ht="24" customHeight="1">
-      <c r="B203" s="10" t="s">
+    <row r="208" spans="1:3" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B208" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="204" spans="1:33" ht="24" customHeight="1">
-      <c r="B204" s="11"/>
-      <c r="AA204" s="6" t="s">
+    <row r="209" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B209" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA209" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB204" s="6" t="s">
+      <c r="AB209" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC204" s="6" t="s">
+      <c r="AC209" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD204" s="6" t="s">
+      <c r="AD209" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE204" s="6" t="s">
+      <c r="AE209" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF204" s="6" t="s">
+      <c r="AF209" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG204" s="6" t="s">
+      <c r="AG209" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="206" spans="1:33" ht="24" customHeight="1">
-      <c r="A206" s="9" t="s">
+    <row r="210" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B210" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA210" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB210" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC210" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD210" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE210" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF210" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG210" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="212" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A212" s="9" t="s">
         <v>356</v>
       </c>
-      <c r="B206" s="9" t="s">
+      <c r="B212" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="207" spans="1:33" ht="24" customHeight="1">
-      <c r="A207" s="14" t="s">
+    <row r="213" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A213" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B207" s="10" t="s">
+      <c r="B213" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C207" s="10" t="s">
+      <c r="C213" s="10" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="208" spans="1:33" ht="24" customHeight="1">
-      <c r="B208" s="8" t="s">
+    <row r="214" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B214" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="209" spans="1:33" ht="178" customHeight="1">
-      <c r="B209" s="11"/>
-    </row>
-    <row r="212" spans="1:33" ht="24" customHeight="1">
-      <c r="A212" s="12" t="s">
+    <row r="215" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B215" s="11" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="218" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A218" s="12" t="s">
         <v>358</v>
       </c>
-      <c r="B212" s="12" t="s">
+      <c r="B218" s="12" t="s">
         <v>359</v>
       </c>
     </row>
-    <row r="213" spans="1:33" ht="24" customHeight="1">
-      <c r="B213" s="13" t="s">
+    <row r="219" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B219" s="13" t="s">
         <v>360</v>
       </c>
     </row>
-    <row r="215" spans="1:33" ht="24" customHeight="1">
-      <c r="A215" s="9" t="s">
+    <row r="221" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A221" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="B215" s="9" t="s">
+      <c r="B221" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="216" spans="1:33" ht="24" customHeight="1">
-      <c r="A216" s="14" t="s">
+    <row r="222" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A222" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B216" s="10" t="s">
+      <c r="B222" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C216" s="10" t="s">
+      <c r="C222" s="10" t="s">
         <v>362</v>
       </c>
     </row>
-    <row r="217" spans="1:33" ht="24" customHeight="1">
-      <c r="B217" s="10" t="s">
+    <row r="223" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B223" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="218" spans="1:33" ht="24" customHeight="1">
-      <c r="B218" s="11"/>
-      <c r="AA218" s="6" t="s">
+    <row r="224" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B224" s="11" t="s">
         <v>246</v>
       </c>
-      <c r="AB218" s="6" t="s">
+      <c r="AA224" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB224" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC218" s="6" t="s">
+      <c r="AC224" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD218" s="6" t="s">
+      <c r="AD224" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE218" s="6" t="s">
+      <c r="AE224" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF218" s="6" t="s">
+      <c r="AF224" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG218" s="6" t="s">
+      <c r="AG224" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="220" spans="1:33" ht="24" customHeight="1">
-      <c r="A220" s="9" t="s">
+    <row r="226" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A226" s="9" t="s">
         <v>363</v>
       </c>
-      <c r="B220" s="9" t="s">
+      <c r="B226" s="9" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="221" spans="1:33" ht="24" customHeight="1">
-      <c r="A221" s="14" t="s">
+    <row r="227" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A227" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B221" s="10" t="s">
+      <c r="B227" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="C221" s="10" t="s">
+      <c r="C227" s="10" t="s">
         <v>366</v>
       </c>
     </row>
-    <row r="222" spans="1:33" ht="24" customHeight="1">
-      <c r="B222" s="11"/>
-      <c r="AA222" s="6" t="s">
+    <row r="228" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B228" s="11"/>
+      <c r="AA228" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB222" s="6" t="s">
+      <c r="AB228" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC222" s="6" t="s">
+      <c r="AC228" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD222" s="6" t="s">
+      <c r="AD228" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE222" s="6" t="s">
+      <c r="AE228" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF222" s="6" t="s">
+      <c r="AF228" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="224" spans="1:33" ht="24" customHeight="1">
-      <c r="A224" s="9" t="s">
+    <row r="230" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A230" s="9" t="s">
         <v>372</v>
       </c>
-      <c r="B224" s="9" t="s">
+      <c r="B230" s="9" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="225" spans="1:33" ht="24" customHeight="1">
-      <c r="A225" s="14" t="s">
+    <row r="231" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A231" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B225" s="10" t="s">
+      <c r="B231" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="C225" s="10" t="s">
+      <c r="C231" s="10" t="s">
         <v>375</v>
       </c>
     </row>
-    <row r="226" spans="1:33" ht="24" customHeight="1">
-      <c r="B226" s="11"/>
-      <c r="AA226" s="6" t="s">
+    <row r="232" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B232" s="11"/>
+      <c r="AA232" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB226" s="6" t="s">
+      <c r="AB232" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC226" s="6" t="s">
+      <c r="AC232" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD226" s="6" t="s">
+      <c r="AD232" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE226" s="6" t="s">
+      <c r="AE232" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF226" s="6" t="s">
+      <c r="AF232" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="228" spans="1:33" ht="24" customHeight="1">
-      <c r="A228" s="9" t="s">
+    <row r="234" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A234" s="9" t="s">
         <v>376</v>
       </c>
-      <c r="B228" s="9" t="s">
+      <c r="B234" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="229" spans="1:33" ht="24" customHeight="1">
-      <c r="A229" s="14" t="s">
+    <row r="235" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A235" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B229" s="10" t="s">
+      <c r="B235" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C229" s="10" t="s">
+      <c r="C235" s="10" t="s">
         <v>377</v>
       </c>
     </row>
-    <row r="230" spans="1:33" ht="24" customHeight="1">
-      <c r="B230" s="8" t="s">
+    <row r="236" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B236" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="231" spans="1:33" ht="178" customHeight="1">
-      <c r="B231" s="11"/>
-    </row>
-    <row r="234" spans="1:33" ht="24" customHeight="1">
-      <c r="A234" s="12" t="s">
+    <row r="237" spans="1:32" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B237" s="11"/>
+    </row>
+    <row r="240" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A240" s="12" t="s">
         <v>378</v>
       </c>
-      <c r="B234" s="12" t="s">
+      <c r="B240" s="12" t="s">
         <v>379</v>
       </c>
     </row>
-    <row r="235" spans="1:33" ht="24" customHeight="1">
-      <c r="B235" s="13" t="s">
+    <row r="241" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B241" s="13" t="s">
         <v>380</v>
       </c>
     </row>
-    <row r="237" spans="1:33" ht="24" customHeight="1">
-      <c r="A237" s="9" t="s">
+    <row r="243" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A243" s="9" t="s">
         <v>381</v>
       </c>
-      <c r="B237" s="9" t="s">
+      <c r="B243" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="238" spans="1:33" ht="24" customHeight="1">
-      <c r="A238" s="14" t="s">
+    <row r="244" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A244" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B238" s="10" t="s">
+      <c r="B244" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C238" s="10" t="s">
+      <c r="C244" s="10" t="s">
         <v>382</v>
       </c>
     </row>
-    <row r="239" spans="1:33" ht="24" customHeight="1">
-      <c r="B239" s="10" t="s">
+    <row r="245" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B245" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="240" spans="1:33" ht="24" customHeight="1">
-      <c r="B240" s="11"/>
-      <c r="AA240" s="6" t="s">
+    <row r="246" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B246" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA246" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB240" s="6" t="s">
+      <c r="AB246" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC240" s="6" t="s">
+      <c r="AC246" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD240" s="6" t="s">
+      <c r="AD246" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE240" s="6" t="s">
+      <c r="AE246" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF240" s="6" t="s">
+      <c r="AF246" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG240" s="6" t="s">
+      <c r="AG246" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="242" spans="1:32" ht="24" customHeight="1">
-      <c r="A242" s="9" t="s">
+    <row r="248" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A248" s="9" t="s">
         <v>383</v>
       </c>
-      <c r="B242" s="9" t="s">
+      <c r="B248" s="9" t="s">
         <v>364</v>
       </c>
     </row>
-    <row r="243" spans="1:32" ht="24" customHeight="1">
-      <c r="A243" s="14" t="s">
+    <row r="249" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A249" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B243" s="10" t="s">
+      <c r="B249" s="10" t="s">
         <v>365</v>
       </c>
-      <c r="C243" s="10" t="s">
+      <c r="C249" s="10" t="s">
         <v>384</v>
       </c>
     </row>
-    <row r="244" spans="1:32" ht="24" customHeight="1">
-      <c r="B244" s="11"/>
-      <c r="AA244" s="6" t="s">
+    <row r="250" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B250" s="11" t="s">
         <v>367</v>
       </c>
-      <c r="AB244" s="6" t="s">
+      <c r="AA250" s="6" t="s">
+        <v>367</v>
+      </c>
+      <c r="AB250" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC244" s="6" t="s">
+      <c r="AC250" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD244" s="6" t="s">
+      <c r="AD250" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE244" s="6" t="s">
+      <c r="AE250" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF244" s="6" t="s">
+      <c r="AF250" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="246" spans="1:32" ht="24" customHeight="1">
-      <c r="A246" s="9" t="s">
+    <row r="252" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A252" s="9" t="s">
         <v>385</v>
       </c>
-      <c r="B246" s="9" t="s">
+      <c r="B252" s="9" t="s">
         <v>373</v>
       </c>
     </row>
-    <row r="247" spans="1:32" ht="24" customHeight="1">
-      <c r="A247" s="14" t="s">
+    <row r="253" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A253" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B247" s="10" t="s">
+      <c r="B253" s="10" t="s">
         <v>374</v>
       </c>
-      <c r="C247" s="10" t="s">
+      <c r="C253" s="10" t="s">
         <v>386</v>
       </c>
     </row>
-    <row r="248" spans="1:32" ht="24" customHeight="1">
-      <c r="B248" s="11"/>
-      <c r="AA248" s="6" t="s">
+    <row r="254" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B254" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="AA254" s="6" t="s">
         <v>367</v>
       </c>
-      <c r="AB248" s="6" t="s">
+      <c r="AB254" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="AC248" s="6" t="s">
+      <c r="AC254" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="AD248" s="6" t="s">
+      <c r="AD254" s="6" t="s">
         <v>370</v>
       </c>
-      <c r="AE248" s="6" t="s">
+      <c r="AE254" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="AF248" s="6" t="s">
+      <c r="AF254" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="250" spans="1:32" ht="24" customHeight="1">
-      <c r="A250" s="9" t="s">
+    <row r="256" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A256" s="9" t="s">
         <v>387</v>
       </c>
-      <c r="B250" s="9" t="s">
+      <c r="B256" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="251" spans="1:32" ht="24" customHeight="1">
-      <c r="A251" s="14" t="s">
+    <row r="257" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A257" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B251" s="10" t="s">
+      <c r="B257" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C251" s="10" t="s">
+      <c r="C257" s="10" t="s">
         <v>388</v>
       </c>
     </row>
-    <row r="252" spans="1:32" ht="24" customHeight="1">
-      <c r="B252" s="8" t="s">
+    <row r="258" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B258" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="253" spans="1:32" ht="178" customHeight="1">
-      <c r="B253" s="11"/>
-    </row>
-    <row r="256" spans="1:32" ht="24" customHeight="1">
-      <c r="A256" s="12" t="s">
+    <row r="259" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B259" s="11"/>
+    </row>
+    <row r="262" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A262" s="12" t="s">
         <v>389</v>
       </c>
-      <c r="B256" s="12" t="s">
+      <c r="B262" s="12" t="s">
         <v>390</v>
       </c>
     </row>
-    <row r="257" spans="1:33" ht="24" customHeight="1">
-      <c r="B257" s="13" t="s">
+    <row r="263" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B263" s="13" t="s">
         <v>391</v>
       </c>
     </row>
-    <row r="259" spans="1:33" ht="24" customHeight="1">
-      <c r="A259" s="9" t="s">
+    <row r="265" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A265" s="9" t="s">
         <v>392</v>
       </c>
-      <c r="B259" s="9" t="s">
+      <c r="B265" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="260" spans="1:33" ht="24" customHeight="1">
-      <c r="A260" s="14" t="s">
+    <row r="266" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A266" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B260" s="10" t="s">
+      <c r="B266" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C260" s="10" t="s">
+      <c r="C266" s="10" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="261" spans="1:33" ht="24" customHeight="1">
-      <c r="B261" s="10" t="s">
+    <row r="267" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B267" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="262" spans="1:33" ht="24" customHeight="1">
-      <c r="B262" s="11"/>
-      <c r="AA262" s="6" t="s">
+    <row r="268" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B268" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA268" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB262" s="6" t="s">
+      <c r="AB268" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC262" s="6" t="s">
+      <c r="AC268" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD262" s="6" t="s">
+      <c r="AD268" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE262" s="6" t="s">
+      <c r="AE268" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF262" s="6" t="s">
+      <c r="AF268" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG262" s="6" t="s">
+      <c r="AG268" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="264" spans="1:33" ht="24" customHeight="1">
-      <c r="A264" s="9" t="s">
+    <row r="269" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B269" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="AA269" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="AB269" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="AC269" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="AD269" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="AE269" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="AF269" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="AG269" s="6" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="271" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A271" s="9" t="s">
         <v>394</v>
       </c>
-      <c r="B264" s="9" t="s">
+      <c r="B271" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="265" spans="1:33" ht="24" customHeight="1">
-      <c r="A265" s="14" t="s">
+    <row r="272" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A272" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B265" s="10" t="s">
+      <c r="B272" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C265" s="10" t="s">
+      <c r="C272" s="10" t="s">
         <v>395</v>
       </c>
     </row>
-    <row r="266" spans="1:33" ht="24" customHeight="1">
-      <c r="B266" s="8" t="s">
+    <row r="273" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B273" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="267" spans="1:33" ht="178" customHeight="1">
-      <c r="B267" s="11"/>
-    </row>
-    <row r="270" spans="1:33" ht="24" customHeight="1">
-      <c r="A270" s="12" t="s">
+    <row r="274" spans="1:33" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B274" s="11" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="277" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A277" s="12" t="s">
         <v>396</v>
       </c>
-      <c r="B270" s="12" t="s">
+      <c r="B277" s="12" t="s">
         <v>397</v>
       </c>
     </row>
-    <row r="271" spans="1:33" ht="24" customHeight="1">
-      <c r="B271" s="13" t="s">
+    <row r="278" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B278" s="13" t="s">
         <v>398</v>
       </c>
     </row>
-    <row r="273" spans="1:33" ht="24" customHeight="1">
-      <c r="A273" s="9" t="s">
+    <row r="280" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A280" s="9" t="s">
         <v>399</v>
       </c>
-      <c r="B273" s="9" t="s">
+      <c r="B280" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="274" spans="1:33" ht="24" customHeight="1">
-      <c r="A274" s="14" t="s">
+    <row r="281" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A281" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B274" s="10" t="s">
+      <c r="B281" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="C274" s="10" t="s">
+      <c r="C281" s="10" t="s">
         <v>400</v>
       </c>
     </row>
-    <row r="275" spans="1:33" ht="24" customHeight="1">
-      <c r="B275" s="10" t="s">
+    <row r="282" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B282" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="276" spans="1:33" ht="24" customHeight="1">
-      <c r="B276" s="11"/>
-      <c r="AA276" s="6" t="s">
+    <row r="283" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B283" s="11" t="s">
+        <v>248</v>
+      </c>
+      <c r="AA283" s="6" t="s">
         <v>246</v>
       </c>
-      <c r="AB276" s="6" t="s">
+      <c r="AB283" s="6" t="s">
         <v>247</v>
       </c>
-      <c r="AC276" s="6" t="s">
+      <c r="AC283" s="6" t="s">
         <v>248</v>
       </c>
-      <c r="AD276" s="6" t="s">
+      <c r="AD283" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="AE276" s="6" t="s">
+      <c r="AE283" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="AF276" s="6" t="s">
+      <c r="AF283" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="AG276" s="6" t="s">
+      <c r="AG283" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="278" spans="1:33" ht="24" customHeight="1">
-      <c r="A278" s="9" t="s">
+    <row r="285" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A285" s="9" t="s">
         <v>401</v>
       </c>
-      <c r="B278" s="9" t="s">
+      <c r="B285" s="9" t="s">
         <v>402</v>
       </c>
     </row>
-    <row r="279" spans="1:33" ht="24" customHeight="1">
-      <c r="A279" s="14" t="s">
+    <row r="286" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A286" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="B279" s="10" t="s">
+      <c r="B286" s="10" t="s">
         <v>403</v>
       </c>
-      <c r="C279" s="10" t="s">
+      <c r="C286" s="10" t="s">
         <v>404</v>
       </c>
     </row>
-    <row r="280" spans="1:33" ht="24" customHeight="1">
-      <c r="B280" s="11"/>
-    </row>
-    <row r="282" spans="1:33" ht="24" customHeight="1">
-      <c r="A282" s="9" t="s">
+    <row r="287" spans="1:33" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B287" s="11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="289" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A289" s="9" t="s">
         <v>405</v>
       </c>
-      <c r="B282" s="9" t="s">
+      <c r="B289" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="283" spans="1:33" ht="24" customHeight="1">
-      <c r="A283" s="14" t="s">
+    <row r="290" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A290" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B283" s="10" t="s">
+      <c r="B290" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C283" s="10" t="s">
+      <c r="C290" s="10" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="284" spans="1:33" ht="24" customHeight="1">
-      <c r="B284" s="8" t="s">
+    <row r="291" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B291" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="285" spans="1:33" ht="178" customHeight="1">
-      <c r="B285" s="11"/>
-    </row>
-    <row r="288" spans="1:33" ht="24" customHeight="1">
-      <c r="A288" s="12" t="s">
+    <row r="292" spans="1:32" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B292" s="11" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="295" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A295" s="12" t="s">
         <v>407</v>
       </c>
-      <c r="B288" s="12" t="s">
+      <c r="B295" s="12" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="289" spans="1:32" ht="24" customHeight="1">
-      <c r="B289" s="13" t="s">
+    <row r="296" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B296" s="13" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="291" spans="1:32" ht="24" customHeight="1">
-      <c r="A291" s="9" t="s">
+    <row r="298" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A298" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="B291" s="9" t="s">
+      <c r="B298" s="9" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="292" spans="1:32" ht="24" customHeight="1">
-      <c r="A292" s="14" t="s">
+    <row r="299" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A299" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="B292" s="10" t="s">
+      <c r="B299" s="10" t="s">
         <v>411</v>
       </c>
-      <c r="C292" s="10" t="s">
+      <c r="C299" s="10" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="293" spans="1:32" ht="24" customHeight="1">
-      <c r="B293" s="10" t="s">
+    <row r="300" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B300" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="294" spans="1:32" ht="24" customHeight="1">
-      <c r="B294" s="11"/>
-      <c r="AA294" s="6" t="s">
+    <row r="301" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B301" s="11" t="s">
+        <v>414</v>
+      </c>
+      <c r="AA301" s="6" t="s">
         <v>413</v>
       </c>
-      <c r="AB294" s="6" t="s">
+      <c r="AB301" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="AC294" s="6" t="s">
+      <c r="AC301" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="AD294" s="6" t="s">
+      <c r="AD301" s="6" t="s">
         <v>416</v>
       </c>
-      <c r="AE294" s="6" t="s">
+      <c r="AE301" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="AF294" s="6" t="s">
+      <c r="AF301" s="6" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="296" spans="1:32" ht="24" customHeight="1">
-      <c r="A296" s="9" t="s">
+    <row r="303" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A303" s="9" t="s">
         <v>418</v>
       </c>
-      <c r="B296" s="9" t="s">
+      <c r="B303" s="9" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="297" spans="1:32" ht="24" customHeight="1">
-      <c r="A297" s="14" t="s">
+    <row r="304" spans="1:32" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A304" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="B297" s="10" t="s">
+      <c r="B304" s="10" t="s">
         <v>254</v>
       </c>
-      <c r="C297" s="10" t="s">
+      <c r="C304" s="10" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="298" spans="1:32" ht="24" customHeight="1">
-      <c r="B298" s="8" t="s">
+    <row r="305" spans="2:2" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B305" s="8" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="299" spans="1:32" ht="178" customHeight="1">
-      <c r="B299" s="11"/>
+    <row r="306" spans="2:2" ht="178" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B306" s="11"/>
     </row>
   </sheetData>
-  <dataValidations count="27">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20">
+  <dataValidations count="4">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B20 B283 B268:B269 B246 B224 B169 B187 B155 B141 B126:B127 B112 B94 B64:B65 B50 B34:B36 B79:B80 B209:B210" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>AA20:AG20</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B34">
-      <formula1>AA34:AG34</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B98" xr:uid="{00000000-0002-0000-0300-000006000000}">
+      <formula1>AA98:AE98</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B48">
-      <formula1>AA48:AG48</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B62">
-      <formula1>AA62:AG62</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B76">
-      <formula1>AA76:AG76</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B90">
-      <formula1>AA90:AG90</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B94">
-      <formula1>AA94:AE94</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B108">
-      <formula1>AA108:AG108</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B122">
-      <formula1>AA122:AG122</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B136">
-      <formula1>AA136:AG136</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B150">
-      <formula1>AA150:AG150</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B164">
-      <formula1>AA164:AG164</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B168">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B173 B287 B195 B191" xr:uid="{00000000-0002-0000-0300-00000C000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B182">
-      <formula1>AA182:AG182</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B186">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B190">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B204">
-      <formula1>AA204:AG204</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B218">
-      <formula1>AA218:AG218</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B222">
-      <formula1>AA222:AF222</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B226">
-      <formula1>AA226:AF226</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B240">
-      <formula1>AA240:AG240</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B244">
-      <formula1>AA244:AF244</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B248">
-      <formula1>AA248:AF248</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B262">
-      <formula1>AA262:AG262</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B276">
-      <formula1>AA276:AG276</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B280">
-      <formula1>"TRUE,FALSE"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B294">
-      <formula1>AA294:AF294</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B228 B301 B254 B250 B232" xr:uid="{00000000-0002-0000-0300-000012000000}">
+      <formula1>AA228:AF228</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>